<commit_message>
updated the R code for the newest dataset
</commit_message>
<xml_diff>
--- a/docs/random/species_table.xlsx
+++ b/docs/random/species_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PhD thesis\Ch4_biodiversity_hotspot_V1\docs\random\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC63A396-8539-423D-87E2-17B0B7910C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B6B6B4-C4EF-407B-8B06-AFFA9EE66997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="species_table" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="303">
   <si>
     <t>order</t>
   </si>
@@ -919,13 +919,16 @@
     <t>Boreal Owl</t>
   </si>
   <si>
-    <t>Lauren's article (common)</t>
-  </si>
-  <si>
-    <t>validated</t>
-  </si>
-  <si>
-    <t>dawn chorus + breeding</t>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>used</t>
+  </si>
+  <si>
+    <t>common_name</t>
+  </si>
+  <si>
+    <t>Lauren_article</t>
   </si>
 </sst>
 </file>
@@ -1933,23 +1936,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C80" zoomScale="107" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G88" sqref="G88"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="121" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="57.85546875" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="5.28515625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="26.5703125" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" customWidth="1"/>
+    <col min="1" max="1" width="35.265625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="57.86328125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="30.265625" customWidth="1"/>
+    <col min="4" max="4" width="26.73046875" customWidth="1"/>
+    <col min="5" max="5" width="22.1328125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="5.265625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="26.59765625" customWidth="1"/>
+    <col min="8" max="8" width="25.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1969,13 +1972,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="H1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1995,7 +1998,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
@@ -2016,7 +2019,7 @@
       </c>
       <c r="H3" s="16"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -2036,7 +2039,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2057,7 +2060,7 @@
       </c>
       <c r="H5" s="16"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
@@ -2077,7 +2080,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="10" t="s">
         <v>5</v>
       </c>
@@ -2098,7 +2101,7 @@
       </c>
       <c r="H7" s="16"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
@@ -2118,7 +2121,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="8" t="s">
         <v>20</v>
       </c>
@@ -2138,7 +2141,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="8" t="s">
         <v>20</v>
       </c>
@@ -2158,7 +2161,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="8" t="s">
         <v>20</v>
       </c>
@@ -2179,7 +2182,7 @@
       </c>
       <c r="H11" s="16"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
@@ -2199,7 +2202,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="8" t="s">
         <v>20</v>
       </c>
@@ -2219,7 +2222,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="8" t="s">
         <v>20</v>
       </c>
@@ -2240,7 +2243,7 @@
       </c>
       <c r="H14" s="16"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="8" t="s">
         <v>20</v>
       </c>
@@ -2260,7 +2263,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="8" t="s">
         <v>20</v>
       </c>
@@ -2280,7 +2283,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
         <v>20</v>
       </c>
@@ -2301,7 +2304,7 @@
       </c>
       <c r="H17" s="16"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="10" t="s">
         <v>20</v>
       </c>
@@ -2322,7 +2325,7 @@
       </c>
       <c r="H18" s="16"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="2" t="s">
         <v>44</v>
       </c>
@@ -2342,7 +2345,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="2" t="s">
         <v>48</v>
       </c>
@@ -2363,7 +2366,7 @@
       </c>
       <c r="H20" s="16"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="5" t="s">
         <v>52</v>
       </c>
@@ -2383,7 +2386,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="8" t="s">
         <v>52</v>
       </c>
@@ -2403,7 +2406,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="8" t="s">
         <v>52</v>
       </c>
@@ -2424,7 +2427,7 @@
       </c>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="8" t="s">
         <v>52</v>
       </c>
@@ -2444,7 +2447,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A25" s="10" t="s">
         <v>52</v>
       </c>
@@ -2464,7 +2467,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A26" s="2" t="s">
         <v>65</v>
       </c>
@@ -2484,7 +2487,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="5" t="s">
         <v>69</v>
       </c>
@@ -2504,7 +2507,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A28" s="10" t="s">
         <v>69</v>
       </c>
@@ -2525,7 +2528,7 @@
       </c>
       <c r="H28" s="16"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="5" t="s">
         <v>75</v>
       </c>
@@ -2545,7 +2548,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="8" t="s">
         <v>75</v>
       </c>
@@ -2565,7 +2568,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="8" t="s">
         <v>75</v>
       </c>
@@ -2585,7 +2588,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="8" t="s">
         <v>83</v>
       </c>
@@ -2606,7 +2609,7 @@
       </c>
       <c r="H32" s="16"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="8" t="s">
         <v>87</v>
       </c>
@@ -2627,7 +2630,7 @@
       </c>
       <c r="H33" s="16"/>
     </row>
-    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A34" s="10" t="s">
         <v>87</v>
       </c>
@@ -2648,7 +2651,7 @@
       </c>
       <c r="H34" s="16"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="5" t="s">
         <v>94</v>
       </c>
@@ -2668,9 +2671,11 @@
         <v>59</v>
       </c>
       <c r="G35" s="1"/>
-      <c r="H35" s="16"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H35" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="8" t="s">
         <v>94</v>
       </c>
@@ -2689,9 +2694,11 @@
       <c r="F36">
         <v>40</v>
       </c>
-      <c r="H36" s="16"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H36" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" s="8" t="s">
         <v>94</v>
       </c>
@@ -2711,9 +2718,11 @@
         <v>61</v>
       </c>
       <c r="G37" s="1"/>
-      <c r="H37" s="17"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H37" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" s="8" t="s">
         <v>94</v>
       </c>
@@ -2733,7 +2742,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39" s="8" t="s">
         <v>94</v>
       </c>
@@ -2753,9 +2762,11 @@
         <v>61</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="16"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H39" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" s="8" t="s">
         <v>94</v>
       </c>
@@ -2775,7 +2786,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41" s="8" t="s">
         <v>94</v>
       </c>
@@ -2795,7 +2806,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" s="8" t="s">
         <v>94</v>
       </c>
@@ -2815,9 +2826,11 @@
         <v>54</v>
       </c>
       <c r="G42" s="1"/>
-      <c r="H42" s="16"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H42" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" s="8" t="s">
         <v>94</v>
       </c>
@@ -2836,9 +2849,11 @@
       <c r="F43">
         <v>30</v>
       </c>
-      <c r="H43" s="16"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H43" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" s="8" t="s">
         <v>94</v>
       </c>
@@ -2858,7 +2873,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" s="8" t="s">
         <v>94</v>
       </c>
@@ -2877,9 +2892,11 @@
       <c r="F45">
         <v>60</v>
       </c>
-      <c r="H45" s="16"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H45" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A46" s="8" t="s">
         <v>94</v>
       </c>
@@ -2899,7 +2916,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A47" s="8" t="s">
         <v>94</v>
       </c>
@@ -2919,7 +2936,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A48" s="8" t="s">
         <v>94</v>
       </c>
@@ -2939,7 +2956,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" s="8" t="s">
         <v>94</v>
       </c>
@@ -2959,7 +2976,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" s="8" t="s">
         <v>94</v>
       </c>
@@ -2979,7 +2996,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" s="8" t="s">
         <v>94</v>
       </c>
@@ -2999,7 +3016,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52" s="8" t="s">
         <v>94</v>
       </c>
@@ -3019,7 +3036,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" s="8" t="s">
         <v>94</v>
       </c>
@@ -3039,7 +3056,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" s="8" t="s">
         <v>94</v>
       </c>
@@ -3058,9 +3075,11 @@
       <c r="F54">
         <v>23</v>
       </c>
-      <c r="H54" s="16"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H54" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" s="8" t="s">
         <v>94</v>
       </c>
@@ -3080,7 +3099,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56" s="8" t="s">
         <v>94</v>
       </c>
@@ -3100,7 +3119,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57" s="8" t="s">
         <v>94</v>
       </c>
@@ -3120,7 +3139,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" s="8" t="s">
         <v>94</v>
       </c>
@@ -3140,9 +3159,11 @@
         <v>57</v>
       </c>
       <c r="G58" s="1"/>
-      <c r="H58" s="16"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H58" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" s="8" t="s">
         <v>94</v>
       </c>
@@ -3161,8 +3182,11 @@
       <c r="F59">
         <v>61</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H59" s="17" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" s="8" t="s">
         <v>94</v>
       </c>
@@ -3182,9 +3206,11 @@
         <v>54</v>
       </c>
       <c r="G60" s="1"/>
-      <c r="H60" s="16"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H60" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" s="8" t="s">
         <v>94</v>
       </c>
@@ -3203,9 +3229,11 @@
       <c r="F61">
         <v>62</v>
       </c>
-      <c r="H61" s="16"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H61" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" s="8" t="s">
         <v>94</v>
       </c>
@@ -3225,9 +3253,11 @@
         <v>62</v>
       </c>
       <c r="G62" s="1"/>
-      <c r="H62" s="17"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H62" s="17" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" s="8" t="s">
         <v>94</v>
       </c>
@@ -3246,9 +3276,11 @@
       <c r="F63">
         <v>61</v>
       </c>
-      <c r="H63" s="16"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H63" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A64" s="8" t="s">
         <v>94</v>
       </c>
@@ -3267,9 +3299,11 @@
       <c r="F64">
         <v>61</v>
       </c>
-      <c r="H64" s="16"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H64" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A65" s="8" t="s">
         <v>94</v>
       </c>
@@ -3289,9 +3323,11 @@
         <v>61</v>
       </c>
       <c r="G65" s="1"/>
-      <c r="H65" s="16"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H65" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A66" s="8" t="s">
         <v>94</v>
       </c>
@@ -3311,9 +3347,11 @@
         <v>58</v>
       </c>
       <c r="G66" s="1"/>
-      <c r="H66" s="17"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H66" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A67" s="8" t="s">
         <v>94</v>
       </c>
@@ -3332,9 +3370,11 @@
       <c r="F67">
         <v>59</v>
       </c>
-      <c r="H67" s="16"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H67" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A68" s="8" t="s">
         <v>94</v>
       </c>
@@ -3354,7 +3394,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A69" s="8" t="s">
         <v>94</v>
       </c>
@@ -3374,9 +3414,11 @@
         <v>60</v>
       </c>
       <c r="G69" s="1"/>
-      <c r="H69" s="16"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H69" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A70" s="8" t="s">
         <v>94</v>
       </c>
@@ -3395,9 +3437,11 @@
       <c r="F70">
         <v>60</v>
       </c>
-      <c r="H70" s="16"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H70" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A71" s="8" t="s">
         <v>94</v>
       </c>
@@ -3417,9 +3461,11 @@
         <v>60</v>
       </c>
       <c r="G71" s="1"/>
-      <c r="H71" s="16"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H71" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A72" s="8" t="s">
         <v>94</v>
       </c>
@@ -3438,9 +3484,11 @@
       <c r="F72">
         <v>42</v>
       </c>
-      <c r="H72" s="16"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H72" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A73" s="8" t="s">
         <v>94</v>
       </c>
@@ -3459,9 +3507,11 @@
       <c r="F73">
         <v>46</v>
       </c>
-      <c r="H73" s="16"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H73" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A74" s="8" t="s">
         <v>94</v>
       </c>
@@ -3481,7 +3531,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A75" s="8" t="s">
         <v>94</v>
       </c>
@@ -3501,9 +3551,11 @@
         <v>60</v>
       </c>
       <c r="G75" s="1"/>
-      <c r="H75" s="16"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H75" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A76" s="8" t="s">
         <v>94</v>
       </c>
@@ -3522,9 +3574,11 @@
       <c r="F76">
         <v>62</v>
       </c>
-      <c r="H76" s="16"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H76" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A77" s="8" t="s">
         <v>94</v>
       </c>
@@ -3544,9 +3598,11 @@
         <v>62</v>
       </c>
       <c r="G77" s="1"/>
-      <c r="H77" s="17"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H77" s="17" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A78" s="8" t="s">
         <v>94</v>
       </c>
@@ -3566,7 +3622,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A79" s="8" t="s">
         <v>94</v>
       </c>
@@ -3586,9 +3642,11 @@
         <v>59</v>
       </c>
       <c r="G79" s="1"/>
-      <c r="H79" s="17"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H79" s="17" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A80" s="8" t="s">
         <v>94</v>
       </c>
@@ -3607,9 +3665,11 @@
       <c r="F80">
         <v>23</v>
       </c>
-      <c r="H80" s="16"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H80" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A81" s="8" t="s">
         <v>94</v>
       </c>
@@ -3629,7 +3689,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A82" s="8" t="s">
         <v>94</v>
       </c>
@@ -3649,7 +3709,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A83" s="8" t="s">
         <v>94</v>
       </c>
@@ -3669,7 +3729,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A84" s="8" t="s">
         <v>94</v>
       </c>
@@ -3689,7 +3749,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A85" s="8" t="s">
         <v>94</v>
       </c>
@@ -3709,9 +3769,11 @@
         <v>61</v>
       </c>
       <c r="G85" s="1"/>
-      <c r="H85" s="16"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H85" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A86" s="8" t="s">
         <v>94</v>
       </c>
@@ -3731,9 +3793,11 @@
         <v>59</v>
       </c>
       <c r="G86" s="1"/>
-      <c r="H86" s="17"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H86" s="17" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A87" s="8" t="s">
         <v>94</v>
       </c>
@@ -3753,9 +3817,11 @@
         <v>61</v>
       </c>
       <c r="G87" s="1"/>
-      <c r="H87" s="17"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H87" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A88" s="8" t="s">
         <v>94</v>
       </c>
@@ -3775,9 +3841,11 @@
         <v>59</v>
       </c>
       <c r="G88" s="1"/>
-      <c r="H88" s="16"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H88" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A89" s="8" t="s">
         <v>94</v>
       </c>
@@ -3797,9 +3865,11 @@
         <v>62</v>
       </c>
       <c r="G89" s="1"/>
-      <c r="H89" s="17"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H89" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A90" s="8" t="s">
         <v>94</v>
       </c>
@@ -3819,9 +3889,11 @@
         <v>61</v>
       </c>
       <c r="G90" s="1"/>
-      <c r="H90" s="17"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H90" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A91" s="8" t="s">
         <v>94</v>
       </c>
@@ -3841,9 +3913,11 @@
         <v>61</v>
       </c>
       <c r="G91" s="1"/>
-      <c r="H91" s="17"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H91" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A92" s="8" t="s">
         <v>94</v>
       </c>
@@ -3863,9 +3937,11 @@
         <v>62</v>
       </c>
       <c r="G92" s="1"/>
-      <c r="H92" s="17"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H92" s="17" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A93" s="8" t="s">
         <v>94</v>
       </c>
@@ -3885,7 +3961,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A94" s="8" t="s">
         <v>94</v>
       </c>
@@ -3905,7 +3981,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A95" s="8" t="s">
         <v>94</v>
       </c>
@@ -3924,8 +4000,11 @@
       <c r="F95">
         <v>62</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H95" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A96" s="8" t="s">
         <v>94</v>
       </c>
@@ -3945,9 +4024,11 @@
         <v>62</v>
       </c>
       <c r="G96" s="1"/>
-      <c r="H96" s="16"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H96" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A97" s="8" t="s">
         <v>94</v>
       </c>
@@ -3967,9 +4048,11 @@
         <v>58</v>
       </c>
       <c r="G97" s="1"/>
-      <c r="H97" s="17"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H97" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A98" s="8" t="s">
         <v>94</v>
       </c>
@@ -3989,9 +4072,11 @@
         <v>58</v>
       </c>
       <c r="G98" s="1"/>
-      <c r="H98" s="16"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H98" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A99" s="8" t="s">
         <v>94</v>
       </c>
@@ -4011,9 +4096,11 @@
         <v>61</v>
       </c>
       <c r="G99" s="1"/>
-      <c r="H99" s="17"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H99" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A100" s="8" t="s">
         <v>94</v>
       </c>
@@ -4035,7 +4122,7 @@
       <c r="G100" s="1"/>
       <c r="H100" s="18"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A101" s="8" t="s">
         <v>94</v>
       </c>
@@ -4055,9 +4142,11 @@
         <v>49</v>
       </c>
       <c r="G101" s="1"/>
-      <c r="H101" s="16"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H101" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A102" s="8" t="s">
         <v>94</v>
       </c>
@@ -4077,7 +4166,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A103" s="8" t="s">
         <v>94</v>
       </c>
@@ -4097,9 +4186,11 @@
         <v>50</v>
       </c>
       <c r="G103" s="1"/>
-      <c r="H103" s="17"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H103" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A104" s="8" t="s">
         <v>94</v>
       </c>
@@ -4118,9 +4209,11 @@
       <c r="F104">
         <v>62</v>
       </c>
-      <c r="H104" s="16"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H104" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A105" s="8" t="s">
         <v>94</v>
       </c>
@@ -4140,7 +4233,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A106" s="10" t="s">
         <v>94</v>
       </c>
@@ -4160,7 +4253,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A107" s="2" t="s">
         <v>257</v>
       </c>
@@ -4180,7 +4273,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A108" s="5" t="s">
         <v>261</v>
       </c>
@@ -4200,7 +4293,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A109" s="8" t="s">
         <v>261</v>
       </c>
@@ -4220,7 +4313,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A110" s="8" t="s">
         <v>261</v>
       </c>
@@ -4240,7 +4333,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A111" s="8" t="s">
         <v>261</v>
       </c>
@@ -4260,7 +4353,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A112" s="8" t="s">
         <v>261</v>
       </c>
@@ -4280,7 +4373,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A113" s="8" t="s">
         <v>261</v>
       </c>
@@ -4300,7 +4393,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A114" s="8" t="s">
         <v>261</v>
       </c>
@@ -4320,7 +4413,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A115" s="10" t="s">
         <v>261</v>
       </c>
@@ -4340,8 +4433,11 @@
         <v>43</v>
       </c>
       <c r="G115" s="1"/>
-    </row>
-    <row r="116" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H115" s="17" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A116" s="2" t="s">
         <v>279</v>
       </c>
@@ -4361,7 +4457,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A117" s="5" t="s">
         <v>283</v>
       </c>
@@ -4380,9 +4476,11 @@
       <c r="F117">
         <v>43</v>
       </c>
-      <c r="H117" s="16"/>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H117" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A118" s="8" t="s">
         <v>283</v>
       </c>
@@ -4402,7 +4500,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A119" s="8" t="s">
         <v>283</v>
       </c>
@@ -4422,7 +4520,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A120" s="8" t="s">
         <v>283</v>
       </c>
@@ -4442,7 +4540,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A121" s="8" t="s">
         <v>283</v>
       </c>
@@ -4462,7 +4560,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A122" s="8" t="s">
         <v>283</v>
       </c>
@@ -4483,7 +4581,7 @@
       </c>
       <c r="G122" s="1"/>
     </row>
-    <row r="123" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A123" s="10" t="s">
         <v>283</v>
       </c>

</xml_diff>

<commit_message>
updated table and R code for 44 species
</commit_message>
<xml_diff>
--- a/docs/random/species_table.xlsx
+++ b/docs/random/species_table.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PhD thesis\Ch4_biodiversity_hotspot_V1\docs\random\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B6B6B4-C4EF-407B-8B06-AFFA9EE66997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A7FACB-DBF6-47B9-8E66-50F23DD1D7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="species_table" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">species_table!$H$1:$H$123</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="303">
   <si>
     <t>order</t>
   </si>
@@ -721,9 +724,6 @@
     <t>Empidonax difficilis</t>
   </si>
   <si>
-    <t>Western Flycatcher</t>
-  </si>
-  <si>
     <t>Empidonax hammondii</t>
   </si>
   <si>
@@ -922,20 +922,23 @@
     <t>Y</t>
   </si>
   <si>
+    <t>common_name</t>
+  </si>
+  <si>
+    <t>Lauren_article</t>
+  </si>
+  <si>
     <t>used</t>
   </si>
   <si>
-    <t>common_name</t>
-  </si>
-  <si>
-    <t>Lauren_article</t>
+    <t>Pacific-slope Flycatcher</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1070,8 +1073,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="38">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1266,18 +1276,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1559,7 +1557,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1577,8 +1575,7 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1936,23 +1933,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="121" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="C72" zoomScale="121" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.265625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="57.86328125" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="30.265625" customWidth="1"/>
-    <col min="4" max="4" width="26.73046875" customWidth="1"/>
-    <col min="5" max="5" width="22.1328125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="5.265625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="26.59765625" customWidth="1"/>
-    <col min="8" max="8" width="25.265625" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="57.85546875" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1963,7 +1960,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -1972,13 +1969,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1998,7 +1995,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
@@ -2019,7 +2016,7 @@
       </c>
       <c r="H3" s="16"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -2039,7 +2036,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2060,7 +2057,7 @@
       </c>
       <c r="H5" s="16"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
@@ -2080,7 +2077,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>5</v>
       </c>
@@ -2101,7 +2098,7 @@
       </c>
       <c r="H7" s="16"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
@@ -2120,8 +2117,9 @@
       <c r="F8">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H8" s="16"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>20</v>
       </c>
@@ -2141,7 +2139,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>20</v>
       </c>
@@ -2161,7 +2159,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>20</v>
       </c>
@@ -2182,7 +2180,7 @@
       </c>
       <c r="H11" s="16"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
@@ -2202,7 +2200,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>20</v>
       </c>
@@ -2222,7 +2220,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>20</v>
       </c>
@@ -2243,7 +2241,7 @@
       </c>
       <c r="H14" s="16"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>20</v>
       </c>
@@ -2263,7 +2261,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>20</v>
       </c>
@@ -2283,7 +2281,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>20</v>
       </c>
@@ -2304,7 +2302,7 @@
       </c>
       <c r="H17" s="16"/>
     </row>
-    <row r="18" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>20</v>
       </c>
@@ -2325,7 +2323,7 @@
       </c>
       <c r="H18" s="16"/>
     </row>
-    <row r="19" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>44</v>
       </c>
@@ -2345,7 +2343,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>48</v>
       </c>
@@ -2366,7 +2364,7 @@
       </c>
       <c r="H20" s="16"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>52</v>
       </c>
@@ -2386,7 +2384,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>52</v>
       </c>
@@ -2406,7 +2404,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>52</v>
       </c>
@@ -2427,7 +2425,7 @@
       </c>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>52</v>
       </c>
@@ -2447,7 +2445,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>52</v>
       </c>
@@ -2467,7 +2465,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>65</v>
       </c>
@@ -2487,7 +2485,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>69</v>
       </c>
@@ -2507,7 +2505,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>69</v>
       </c>
@@ -2528,7 +2526,7 @@
       </c>
       <c r="H28" s="16"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>75</v>
       </c>
@@ -2548,7 +2546,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>75</v>
       </c>
@@ -2568,7 +2566,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>75</v>
       </c>
@@ -2588,7 +2586,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>83</v>
       </c>
@@ -2609,7 +2607,7 @@
       </c>
       <c r="H32" s="16"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>87</v>
       </c>
@@ -2630,7 +2628,7 @@
       </c>
       <c r="H33" s="16"/>
     </row>
-    <row r="34" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>87</v>
       </c>
@@ -2651,7 +2649,7 @@
       </c>
       <c r="H34" s="16"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>94</v>
       </c>
@@ -2672,10 +2670,10 @@
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>94</v>
       </c>
@@ -2695,10 +2693,10 @@
         <v>40</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>94</v>
       </c>
@@ -2719,10 +2717,10 @@
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>94</v>
       </c>
@@ -2742,7 +2740,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>94</v>
       </c>
@@ -2763,10 +2761,10 @@
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>94</v>
       </c>
@@ -2786,7 +2784,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>94</v>
       </c>
@@ -2806,7 +2804,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>94</v>
       </c>
@@ -2827,10 +2825,10 @@
       </c>
       <c r="G42" s="1"/>
       <c r="H42" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>94</v>
       </c>
@@ -2850,10 +2848,10 @@
         <v>30</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>94</v>
       </c>
@@ -2873,7 +2871,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>94</v>
       </c>
@@ -2893,10 +2891,10 @@
         <v>60</v>
       </c>
       <c r="H45" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>94</v>
       </c>
@@ -2916,7 +2914,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>94</v>
       </c>
@@ -2936,7 +2934,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>94</v>
       </c>
@@ -2956,7 +2954,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>94</v>
       </c>
@@ -2976,7 +2974,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>94</v>
       </c>
@@ -2996,7 +2994,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>94</v>
       </c>
@@ -3016,7 +3014,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>94</v>
       </c>
@@ -3036,7 +3034,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>94</v>
       </c>
@@ -3056,7 +3054,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>94</v>
       </c>
@@ -3076,10 +3074,10 @@
         <v>23</v>
       </c>
       <c r="H54" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>94</v>
       </c>
@@ -3099,7 +3097,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>94</v>
       </c>
@@ -3119,7 +3117,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>94</v>
       </c>
@@ -3139,7 +3137,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>94</v>
       </c>
@@ -3160,10 +3158,10 @@
       </c>
       <c r="G58" s="1"/>
       <c r="H58" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
         <v>94</v>
       </c>
@@ -3182,11 +3180,11 @@
       <c r="F59">
         <v>61</v>
       </c>
-      <c r="H59" s="17" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H59" s="16" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>94</v>
       </c>
@@ -3207,10 +3205,10 @@
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>94</v>
       </c>
@@ -3230,10 +3228,10 @@
         <v>62</v>
       </c>
       <c r="H61" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>94</v>
       </c>
@@ -3253,11 +3251,11 @@
         <v>62</v>
       </c>
       <c r="G62" s="1"/>
-      <c r="H62" s="17" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H62" s="16" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>94</v>
       </c>
@@ -3277,10 +3275,10 @@
         <v>61</v>
       </c>
       <c r="H63" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>94</v>
       </c>
@@ -3300,10 +3298,10 @@
         <v>61</v>
       </c>
       <c r="H64" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>94</v>
       </c>
@@ -3324,10 +3322,10 @@
       </c>
       <c r="G65" s="1"/>
       <c r="H65" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
         <v>94</v>
       </c>
@@ -3348,10 +3346,10 @@
       </c>
       <c r="G66" s="1"/>
       <c r="H66" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
         <v>94</v>
       </c>
@@ -3371,10 +3369,10 @@
         <v>59</v>
       </c>
       <c r="H67" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>94</v>
       </c>
@@ -3394,7 +3392,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
         <v>94</v>
       </c>
@@ -3415,10 +3413,10 @@
       </c>
       <c r="G69" s="1"/>
       <c r="H69" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
         <v>94</v>
       </c>
@@ -3438,10 +3436,10 @@
         <v>60</v>
       </c>
       <c r="H70" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>94</v>
       </c>
@@ -3462,10 +3460,10 @@
       </c>
       <c r="G71" s="1"/>
       <c r="H71" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
         <v>94</v>
       </c>
@@ -3485,10 +3483,10 @@
         <v>42</v>
       </c>
       <c r="H72" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
         <v>94</v>
       </c>
@@ -3508,10 +3506,10 @@
         <v>46</v>
       </c>
       <c r="H73" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
         <v>94</v>
       </c>
@@ -3530,8 +3528,11 @@
       <c r="F74">
         <v>54</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H74" s="16" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
         <v>94</v>
       </c>
@@ -3552,10 +3553,10 @@
       </c>
       <c r="G75" s="1"/>
       <c r="H75" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
         <v>94</v>
       </c>
@@ -3575,10 +3576,10 @@
         <v>62</v>
       </c>
       <c r="H76" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
         <v>94</v>
       </c>
@@ -3598,11 +3599,11 @@
         <v>62</v>
       </c>
       <c r="G77" s="1"/>
-      <c r="H77" s="17" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H77" s="16" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
         <v>94</v>
       </c>
@@ -3622,7 +3623,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
         <v>94</v>
       </c>
@@ -3642,11 +3643,9 @@
         <v>59</v>
       </c>
       <c r="G79" s="1"/>
-      <c r="H79" s="17" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H79" s="17"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
         <v>94</v>
       </c>
@@ -3666,10 +3665,10 @@
         <v>23</v>
       </c>
       <c r="H80" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
         <v>94</v>
       </c>
@@ -3689,7 +3688,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
         <v>94</v>
       </c>
@@ -3709,7 +3708,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
         <v>94</v>
       </c>
@@ -3729,7 +3728,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
         <v>94</v>
       </c>
@@ -3749,7 +3748,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
         <v>94</v>
       </c>
@@ -3770,10 +3769,10 @@
       </c>
       <c r="G85" s="1"/>
       <c r="H85" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
         <v>94</v>
       </c>
@@ -3793,11 +3792,11 @@
         <v>59</v>
       </c>
       <c r="G86" s="1"/>
-      <c r="H86" s="17" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H86" s="16" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
         <v>94</v>
       </c>
@@ -3818,10 +3817,10 @@
       </c>
       <c r="G87" s="1"/>
       <c r="H87" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="8" t="s">
         <v>94</v>
       </c>
@@ -3842,10 +3841,10 @@
       </c>
       <c r="G88" s="1"/>
       <c r="H88" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
         <v>94</v>
       </c>
@@ -3866,10 +3865,10 @@
       </c>
       <c r="G89" s="1"/>
       <c r="H89" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
         <v>94</v>
       </c>
@@ -3890,10 +3889,10 @@
       </c>
       <c r="G90" s="1"/>
       <c r="H90" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
         <v>94</v>
       </c>
@@ -3914,10 +3913,10 @@
       </c>
       <c r="G91" s="1"/>
       <c r="H91" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
         <v>94</v>
       </c>
@@ -3937,11 +3936,11 @@
         <v>62</v>
       </c>
       <c r="G92" s="1"/>
-      <c r="H92" s="17" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H92" s="16" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
         <v>94</v>
       </c>
@@ -3961,7 +3960,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
         <v>94</v>
       </c>
@@ -3981,7 +3980,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
         <v>94</v>
       </c>
@@ -3992,7 +3991,7 @@
         <v>232</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>233</v>
+        <v>302</v>
       </c>
       <c r="E95">
         <v>12474</v>
@@ -4001,10 +4000,10 @@
         <v>62</v>
       </c>
       <c r="H95" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
         <v>94</v>
       </c>
@@ -4012,10 +4011,10 @@
         <v>231</v>
       </c>
       <c r="C96" t="s">
+        <v>233</v>
+      </c>
+      <c r="D96" s="14" t="s">
         <v>234</v>
-      </c>
-      <c r="D96" s="14" t="s">
-        <v>235</v>
       </c>
       <c r="E96">
         <v>141949</v>
@@ -4025,10 +4024,10 @@
       </c>
       <c r="G96" s="1"/>
       <c r="H96" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
         <v>94</v>
       </c>
@@ -4036,10 +4035,10 @@
         <v>231</v>
       </c>
       <c r="C97" t="s">
+        <v>235</v>
+      </c>
+      <c r="D97" s="14" t="s">
         <v>236</v>
-      </c>
-      <c r="D97" s="14" t="s">
-        <v>237</v>
       </c>
       <c r="E97">
         <v>44654</v>
@@ -4049,10 +4048,10 @@
       </c>
       <c r="G97" s="1"/>
       <c r="H97" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
         <v>94</v>
       </c>
@@ -4060,10 +4059,10 @@
         <v>231</v>
       </c>
       <c r="C98" t="s">
+        <v>237</v>
+      </c>
+      <c r="D98" s="14" t="s">
         <v>238</v>
-      </c>
-      <c r="D98" s="14" t="s">
-        <v>239</v>
       </c>
       <c r="E98">
         <v>9356</v>
@@ -4073,10 +4072,10 @@
       </c>
       <c r="G98" s="1"/>
       <c r="H98" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
         <v>94</v>
       </c>
@@ -4084,10 +4083,10 @@
         <v>231</v>
       </c>
       <c r="C99" t="s">
+        <v>239</v>
+      </c>
+      <c r="D99" s="14" t="s">
         <v>240</v>
-      </c>
-      <c r="D99" s="14" t="s">
-        <v>241</v>
       </c>
       <c r="E99">
         <v>17061</v>
@@ -4097,10 +4096,10 @@
       </c>
       <c r="G99" s="1"/>
       <c r="H99" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
         <v>94</v>
       </c>
@@ -4108,10 +4107,10 @@
         <v>231</v>
       </c>
       <c r="C100" t="s">
+        <v>241</v>
+      </c>
+      <c r="D100" s="9" t="s">
         <v>242</v>
-      </c>
-      <c r="D100" s="9" t="s">
-        <v>243</v>
       </c>
       <c r="E100">
         <v>5815</v>
@@ -4120,9 +4119,8 @@
         <v>61</v>
       </c>
       <c r="G100" s="1"/>
-      <c r="H100" s="18"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
         <v>94</v>
       </c>
@@ -4130,10 +4128,10 @@
         <v>231</v>
       </c>
       <c r="C101" t="s">
+        <v>243</v>
+      </c>
+      <c r="D101" s="14" t="s">
         <v>244</v>
-      </c>
-      <c r="D101" s="14" t="s">
-        <v>245</v>
       </c>
       <c r="E101">
         <v>21412</v>
@@ -4143,10 +4141,10 @@
       </c>
       <c r="G101" s="1"/>
       <c r="H101" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
         <v>94</v>
       </c>
@@ -4154,10 +4152,10 @@
         <v>231</v>
       </c>
       <c r="C102" t="s">
+        <v>245</v>
+      </c>
+      <c r="D102" s="9" t="s">
         <v>246</v>
-      </c>
-      <c r="D102" s="9" t="s">
-        <v>247</v>
       </c>
       <c r="E102">
         <v>48</v>
@@ -4166,7 +4164,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
         <v>94</v>
       </c>
@@ -4174,10 +4172,10 @@
         <v>231</v>
       </c>
       <c r="C103" t="s">
+        <v>247</v>
+      </c>
+      <c r="D103" s="14" t="s">
         <v>248</v>
-      </c>
-      <c r="D103" s="14" t="s">
-        <v>249</v>
       </c>
       <c r="E103">
         <v>10992</v>
@@ -4187,21 +4185,21 @@
       </c>
       <c r="G103" s="1"/>
       <c r="H103" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
         <v>94</v>
       </c>
       <c r="B104" t="s">
+        <v>249</v>
+      </c>
+      <c r="C104" t="s">
         <v>250</v>
       </c>
-      <c r="C104" t="s">
+      <c r="D104" s="14" t="s">
         <v>251</v>
-      </c>
-      <c r="D104" s="14" t="s">
-        <v>252</v>
       </c>
       <c r="E104">
         <v>87002</v>
@@ -4210,21 +4208,21 @@
         <v>62</v>
       </c>
       <c r="H104" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.45">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
         <v>94</v>
       </c>
       <c r="B105" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C105" t="s">
+        <v>252</v>
+      </c>
+      <c r="D105" s="14" t="s">
         <v>253</v>
-      </c>
-      <c r="D105" s="14" t="s">
-        <v>254</v>
       </c>
       <c r="E105">
         <v>6188</v>
@@ -4233,18 +4231,18 @@
         <v>55</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="10" t="s">
         <v>94</v>
       </c>
       <c r="B106" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C106" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="D106" s="15" t="s">
         <v>255</v>
-      </c>
-      <c r="D106" s="15" t="s">
-        <v>256</v>
       </c>
       <c r="E106">
         <v>600</v>
@@ -4253,18 +4251,18 @@
         <v>35</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B107" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="C107" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="C107" s="3" t="s">
+      <c r="D107" s="4" t="s">
         <v>259</v>
-      </c>
-      <c r="D107" s="4" t="s">
-        <v>260</v>
       </c>
       <c r="E107">
         <v>359</v>
@@ -4273,18 +4271,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="B108" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="B108" s="6" t="s">
+      <c r="C108" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="C108" s="6" t="s">
+      <c r="D108" s="7" t="s">
         <v>263</v>
-      </c>
-      <c r="D108" s="7" t="s">
-        <v>264</v>
       </c>
       <c r="E108">
         <v>5261</v>
@@ -4293,18 +4291,18 @@
         <v>57</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="B109" t="s">
         <v>261</v>
       </c>
-      <c r="B109" t="s">
-        <v>262</v>
-      </c>
       <c r="C109" t="s">
+        <v>264</v>
+      </c>
+      <c r="D109" s="9" t="s">
         <v>265</v>
-      </c>
-      <c r="D109" s="9" t="s">
-        <v>266</v>
       </c>
       <c r="E109">
         <v>5182</v>
@@ -4313,18 +4311,18 @@
         <v>57</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="B110" t="s">
         <v>261</v>
       </c>
-      <c r="B110" t="s">
-        <v>262</v>
-      </c>
       <c r="C110" t="s">
+        <v>266</v>
+      </c>
+      <c r="D110" s="9" t="s">
         <v>267</v>
-      </c>
-      <c r="D110" s="9" t="s">
-        <v>268</v>
       </c>
       <c r="E110">
         <v>2928</v>
@@ -4333,18 +4331,18 @@
         <v>60</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="B111" t="s">
         <v>261</v>
       </c>
-      <c r="B111" t="s">
-        <v>262</v>
-      </c>
       <c r="C111" t="s">
+        <v>268</v>
+      </c>
+      <c r="D111" s="9" t="s">
         <v>269</v>
-      </c>
-      <c r="D111" s="9" t="s">
-        <v>270</v>
       </c>
       <c r="E111">
         <v>6417</v>
@@ -4353,18 +4351,18 @@
         <v>62</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="B112" t="s">
         <v>261</v>
       </c>
-      <c r="B112" t="s">
-        <v>262</v>
-      </c>
       <c r="C112" t="s">
+        <v>270</v>
+      </c>
+      <c r="D112" s="9" t="s">
         <v>271</v>
-      </c>
-      <c r="D112" s="9" t="s">
-        <v>272</v>
       </c>
       <c r="E112">
         <v>1589</v>
@@ -4373,18 +4371,18 @@
         <v>54</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="B113" t="s">
         <v>261</v>
       </c>
-      <c r="B113" t="s">
-        <v>262</v>
-      </c>
       <c r="C113" t="s">
+        <v>272</v>
+      </c>
+      <c r="D113" s="9" t="s">
         <v>273</v>
-      </c>
-      <c r="D113" s="9" t="s">
-        <v>274</v>
       </c>
       <c r="E113">
         <v>1910</v>
@@ -4393,18 +4391,18 @@
         <v>56</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="B114" t="s">
         <v>261</v>
       </c>
-      <c r="B114" t="s">
-        <v>262</v>
-      </c>
       <c r="C114" t="s">
+        <v>274</v>
+      </c>
+      <c r="D114" s="9" t="s">
         <v>275</v>
-      </c>
-      <c r="D114" s="9" t="s">
-        <v>276</v>
       </c>
       <c r="E114">
         <v>331</v>
@@ -4413,18 +4411,18 @@
         <v>49</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="B115" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="B115" s="11" t="s">
-        <v>262</v>
-      </c>
       <c r="C115" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="D115" s="12" t="s">
         <v>277</v>
-      </c>
-      <c r="D115" s="12" t="s">
-        <v>278</v>
       </c>
       <c r="E115">
         <v>950</v>
@@ -4433,22 +4431,20 @@
         <v>43</v>
       </c>
       <c r="G115" s="1"/>
-      <c r="H115" s="17" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="H115" s="17"/>
+    </row>
+    <row r="116" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B116" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="C116" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="C116" s="3" t="s">
+      <c r="D116" s="4" t="s">
         <v>281</v>
-      </c>
-      <c r="D116" s="4" t="s">
-        <v>282</v>
       </c>
       <c r="E116">
         <v>26</v>
@@ -4457,18 +4453,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B117" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="B117" s="6" t="s">
+      <c r="C117" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="C117" s="6" t="s">
+      <c r="D117" s="7" t="s">
         <v>285</v>
-      </c>
-      <c r="D117" s="7" t="s">
-        <v>286</v>
       </c>
       <c r="E117">
         <v>498</v>
@@ -4476,22 +4472,20 @@
       <c r="F117">
         <v>43</v>
       </c>
-      <c r="H117" s="16" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H117" s="16"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B118" t="s">
         <v>283</v>
       </c>
-      <c r="B118" t="s">
-        <v>284</v>
-      </c>
       <c r="C118" t="s">
+        <v>286</v>
+      </c>
+      <c r="D118" s="9" t="s">
         <v>287</v>
-      </c>
-      <c r="D118" s="9" t="s">
-        <v>288</v>
       </c>
       <c r="E118">
         <v>4902</v>
@@ -4500,18 +4494,18 @@
         <v>57</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B119" t="s">
         <v>283</v>
       </c>
-      <c r="B119" t="s">
-        <v>284</v>
-      </c>
       <c r="C119" t="s">
+        <v>288</v>
+      </c>
+      <c r="D119" s="9" t="s">
         <v>289</v>
-      </c>
-      <c r="D119" s="9" t="s">
-        <v>290</v>
       </c>
       <c r="E119">
         <v>294</v>
@@ -4520,18 +4514,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B120" t="s">
         <v>283</v>
       </c>
-      <c r="B120" t="s">
-        <v>284</v>
-      </c>
       <c r="C120" t="s">
+        <v>290</v>
+      </c>
+      <c r="D120" s="9" t="s">
         <v>291</v>
-      </c>
-      <c r="D120" s="9" t="s">
-        <v>292</v>
       </c>
       <c r="E120">
         <v>419</v>
@@ -4540,18 +4534,18 @@
         <v>36</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B121" t="s">
         <v>283</v>
       </c>
-      <c r="B121" t="s">
-        <v>284</v>
-      </c>
       <c r="C121" t="s">
+        <v>292</v>
+      </c>
+      <c r="D121" s="9" t="s">
         <v>293</v>
-      </c>
-      <c r="D121" s="9" t="s">
-        <v>294</v>
       </c>
       <c r="E121">
         <v>2223</v>
@@ -4560,18 +4554,18 @@
         <v>54</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B122" t="s">
         <v>283</v>
       </c>
-      <c r="B122" t="s">
-        <v>284</v>
-      </c>
       <c r="C122" t="s">
+        <v>294</v>
+      </c>
+      <c r="D122" s="9" t="s">
         <v>295</v>
-      </c>
-      <c r="D122" s="9" t="s">
-        <v>296</v>
       </c>
       <c r="E122">
         <v>876</v>
@@ -4581,18 +4575,18 @@
       </c>
       <c r="G122" s="1"/>
     </row>
-    <row r="123" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="B123" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="B123" s="11" t="s">
-        <v>284</v>
-      </c>
       <c r="C123" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="D123" s="12" t="s">
         <v>297</v>
-      </c>
-      <c r="D123" s="12" t="s">
-        <v>298</v>
       </c>
       <c r="E123">
         <v>5826</v>
@@ -4602,6 +4596,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="H1:H123" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>